<commit_message>
01.07.2020 MC Sales Details
</commit_message>
<xml_diff>
--- a/2020/July/All Details/01.07.2020/MC Balance Transfer July 2020.xlsx
+++ b/2020/July/All Details/01.07.2020/MC Balance Transfer July 2020.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="96">
   <si>
     <t>Date</t>
   </si>
@@ -633,7 +633,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="157">
+  <cellXfs count="154">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1038,14 +1038,14 @@
     <xf numFmtId="2" fontId="5" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1091,15 +1091,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1138,7 +1129,7 @@
         <xdr:cNvPr id="1317" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{AEF7B42F-C37B-44F8-8D5A-2ED7FEE15E8A}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AEF7B42F-C37B-44F8-8D5A-2ED7FEE15E8A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1150,7 +1141,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -1173,14 +1164,14 @@
         </a:ln>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
             </a14:hiddenFill>
           </a:ext>
           <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
+            <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -1488,9 +1479,9 @@
   <dimension ref="A1:BI231"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="4" topLeftCell="A95" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="I1" sqref="I1"/>
-      <selection pane="bottomLeft" activeCell="B103" sqref="B103"/>
+      <selection pane="bottomLeft" activeCell="E111" sqref="E111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -1775,15 +1766,17 @@
         <v>93</v>
       </c>
       <c r="B5" s="104">
-        <v>0</v>
+        <v>349730</v>
       </c>
       <c r="C5" s="104">
-        <v>0</v>
-      </c>
-      <c r="D5" s="104"/>
+        <v>341910</v>
+      </c>
+      <c r="D5" s="104">
+        <v>150</v>
+      </c>
       <c r="E5" s="104">
         <f>C5+D5</f>
-        <v>0</v>
+        <v>342060</v>
       </c>
       <c r="F5" s="106"/>
       <c r="G5" s="17"/>
@@ -3684,23 +3677,23 @@
       </c>
       <c r="B33" s="2">
         <f>SUM(B5:B32)</f>
-        <v>0</v>
+        <v>349730</v>
       </c>
       <c r="C33" s="2">
         <f>SUM(C5:C32)</f>
-        <v>0</v>
+        <v>341910</v>
       </c>
       <c r="D33" s="2">
         <f>SUM(D5:D32)</f>
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="E33" s="2">
         <f>SUM(E5:E32)</f>
-        <v>0</v>
+        <v>342060</v>
       </c>
       <c r="F33" s="67">
         <f>B33-E33</f>
-        <v>0</v>
+        <v>7670</v>
       </c>
       <c r="G33" s="81"/>
       <c r="H33" s="86"/>
@@ -3971,10 +3964,10 @@
         <v>23</v>
       </c>
       <c r="C37" s="2">
-        <v>6800</v>
+        <v>4000</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>68</v>
+        <v>93</v>
       </c>
       <c r="E37" s="6"/>
       <c r="F37" s="95"/>
@@ -4042,10 +4035,10 @@
         <v>23</v>
       </c>
       <c r="C38" s="2">
-        <v>9500</v>
+        <v>6000</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>61</v>
+        <v>93</v>
       </c>
       <c r="E38" s="3"/>
       <c r="F38" s="67"/>
@@ -4113,10 +4106,10 @@
         <v>23</v>
       </c>
       <c r="C39" s="2">
-        <v>9500</v>
+        <v>6500</v>
       </c>
       <c r="D39" s="122" t="s">
-        <v>60</v>
+        <v>93</v>
       </c>
       <c r="E39" s="3"/>
       <c r="F39" s="95"/>
@@ -4184,10 +4177,10 @@
         <v>33</v>
       </c>
       <c r="C40" s="2">
-        <v>9670</v>
+        <v>5000</v>
       </c>
       <c r="D40" s="122" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="E40" s="3"/>
       <c r="F40" s="95"/>
@@ -4248,18 +4241,10 @@
       <c r="BI40" s="7"/>
     </row>
     <row r="41" spans="1:61" ht="12.6" customHeight="1">
-      <c r="A41" s="136" t="s">
-        <v>57</v>
-      </c>
-      <c r="B41" s="137" t="s">
-        <v>59</v>
-      </c>
-      <c r="C41" s="138">
-        <v>1770</v>
-      </c>
-      <c r="D41" s="137" t="s">
-        <v>56</v>
-      </c>
+      <c r="A41" s="123"/>
+      <c r="B41" s="1"/>
+      <c r="C41" s="2"/>
+      <c r="D41" s="1"/>
       <c r="E41" s="18"/>
       <c r="F41" s="95"/>
       <c r="G41" s="83"/>
@@ -4586,13 +4571,13 @@
       <c r="BI45" s="7"/>
     </row>
     <row r="46" spans="1:61" ht="12" customHeight="1" thickTop="1">
-      <c r="A46" s="154" t="s">
+      <c r="A46" s="136" t="s">
         <v>76</v>
       </c>
-      <c r="B46" s="155" t="s">
+      <c r="B46" s="137" t="s">
         <v>81</v>
       </c>
-      <c r="C46" s="156">
+      <c r="C46" s="138">
         <v>5200</v>
       </c>
       <c r="D46" s="135" t="s">
@@ -5503,10 +5488,10 @@
       </c>
       <c r="B59" s="30"/>
       <c r="C59" s="71">
-        <v>266260</v>
+        <v>270280</v>
       </c>
       <c r="D59" s="72" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="E59" s="3"/>
       <c r="F59" s="30"/>
@@ -5787,10 +5772,10 @@
       </c>
       <c r="B63" s="70"/>
       <c r="C63" s="134">
-        <v>222350</v>
+        <v>201550</v>
       </c>
       <c r="D63" s="70" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="E63" s="3"/>
       <c r="F63" s="48"/>
@@ -5869,10 +5854,10 @@
       </c>
       <c r="B64" s="30"/>
       <c r="C64" s="71">
-        <v>416290</v>
+        <v>454850</v>
       </c>
       <c r="D64" s="72" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="E64" s="3"/>
       <c r="F64" s="50"/>
@@ -5951,10 +5936,10 @@
       </c>
       <c r="B65" s="30"/>
       <c r="C65" s="71">
-        <v>190525</v>
+        <v>192155</v>
       </c>
       <c r="D65" s="70" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="E65" s="3"/>
       <c r="F65" s="48"/>
@@ -8510,7 +8495,7 @@
       <c r="B98" s="145"/>
       <c r="C98" s="32">
         <f>SUM(C37:C97)</f>
-        <v>2072663</v>
+        <v>2080333</v>
       </c>
       <c r="D98" s="28"/>
       <c r="F98" s="110"/>
@@ -8665,7 +8650,7 @@
       <c r="B100" s="143"/>
       <c r="C100" s="29">
         <f>C98+L121</f>
-        <v>2072663</v>
+        <v>2080333</v>
       </c>
       <c r="D100" s="21"/>
       <c r="F100" s="48"/>

</xml_diff>